<commit_message>
fix data for BL8 inv for 13/2/2024
</commit_message>
<xml_diff>
--- a/data/s1/2024/2/13/S1_BL8/13_02_2024-S1_BL8.xlsx
+++ b/data/s1/2024/2/13/S1_BL8/13_02_2024-S1_BL8.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AM742"/>
+  <dimension ref="A1:AM749"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -87318,6 +87318,825 @@
       <c r="AL742" t="inlineStr"/>
       <c r="AM742" t="inlineStr"/>
     </row>
+    <row r="743">
+      <c r="A743" s="1" t="n">
+        <v>45335.75178240741</v>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C743" t="n">
+        <v>472</v>
+      </c>
+      <c r="D743" t="n">
+        <v>555.3</v>
+      </c>
+      <c r="E743" t="n">
+        <v>416</v>
+      </c>
+      <c r="F743" t="n">
+        <v>378.8</v>
+      </c>
+      <c r="G743" t="n">
+        <v>0</v>
+      </c>
+      <c r="H743" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I743" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J743" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="K743" t="n">
+        <v>223</v>
+      </c>
+      <c r="L743" t="n">
+        <v>222.4</v>
+      </c>
+      <c r="M743" t="n">
+        <v>224.4</v>
+      </c>
+      <c r="N743" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="O743" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="P743" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="Q743" t="n">
+        <v>59.98</v>
+      </c>
+      <c r="R743" t="n">
+        <v>59.98</v>
+      </c>
+      <c r="S743" t="n">
+        <v>59.98</v>
+      </c>
+      <c r="T743" t="n">
+        <v>357</v>
+      </c>
+      <c r="U743" t="n">
+        <v>1</v>
+      </c>
+      <c r="V743" t="n">
+        <v>32.3</v>
+      </c>
+      <c r="W743" t="n">
+        <v>39047</v>
+      </c>
+      <c r="X743" t="n">
+        <v>2546</v>
+      </c>
+      <c r="Y743" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z743" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA743" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB743" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC743" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD743" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE743" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF743" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG743" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH743" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI743" t="n">
+        <v>54</v>
+      </c>
+      <c r="AJ743" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK743" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL743" t="inlineStr"/>
+      <c r="AM743" t="inlineStr"/>
+    </row>
+    <row r="744">
+      <c r="A744" s="1" t="n">
+        <v>45335.75525462963</v>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C744" t="n">
+        <v>199.9</v>
+      </c>
+      <c r="D744" t="n">
+        <v>469.1</v>
+      </c>
+      <c r="E744" t="n">
+        <v>370</v>
+      </c>
+      <c r="F744" t="n">
+        <v>303.2</v>
+      </c>
+      <c r="G744" t="n">
+        <v>0</v>
+      </c>
+      <c r="H744" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I744" t="n">
+        <v>0</v>
+      </c>
+      <c r="J744" t="n">
+        <v>0</v>
+      </c>
+      <c r="K744" t="n">
+        <v>222</v>
+      </c>
+      <c r="L744" t="n">
+        <v>221.6</v>
+      </c>
+      <c r="M744" t="n">
+        <v>223.8</v>
+      </c>
+      <c r="N744" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="O744" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="P744" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="Q744" t="n">
+        <v>59.96</v>
+      </c>
+      <c r="R744" t="n">
+        <v>59.96</v>
+      </c>
+      <c r="S744" t="n">
+        <v>59.96</v>
+      </c>
+      <c r="T744" t="n">
+        <v>209</v>
+      </c>
+      <c r="U744" t="n">
+        <v>1</v>
+      </c>
+      <c r="V744" t="n">
+        <v>32.2</v>
+      </c>
+      <c r="W744" t="n">
+        <v>39047.1</v>
+      </c>
+      <c r="X744" t="n">
+        <v>2546</v>
+      </c>
+      <c r="Y744" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z744" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA744" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB744" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC744" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD744" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE744" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF744" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG744" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH744" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI744" t="n">
+        <v>54</v>
+      </c>
+      <c r="AJ744" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK744" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL744" t="inlineStr"/>
+      <c r="AM744" t="inlineStr"/>
+    </row>
+    <row r="745">
+      <c r="A745" s="1" t="n">
+        <v>45335.75873842592</v>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C745" t="n">
+        <v>199.7</v>
+      </c>
+      <c r="D745" t="n">
+        <v>428.1</v>
+      </c>
+      <c r="E745" t="n">
+        <v>199.7</v>
+      </c>
+      <c r="F745" t="n">
+        <v>200.4</v>
+      </c>
+      <c r="G745" t="n">
+        <v>0</v>
+      </c>
+      <c r="H745" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I745" t="n">
+        <v>0</v>
+      </c>
+      <c r="J745" t="n">
+        <v>0</v>
+      </c>
+      <c r="K745" t="n">
+        <v>221.8</v>
+      </c>
+      <c r="L745" t="n">
+        <v>221.6</v>
+      </c>
+      <c r="M745" t="n">
+        <v>223.2</v>
+      </c>
+      <c r="N745" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="O745" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="P745" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="Q745" t="n">
+        <v>59.92</v>
+      </c>
+      <c r="R745" t="n">
+        <v>59.92</v>
+      </c>
+      <c r="S745" t="n">
+        <v>59.92</v>
+      </c>
+      <c r="T745" t="n">
+        <v>61</v>
+      </c>
+      <c r="U745" t="n">
+        <v>1</v>
+      </c>
+      <c r="V745" t="n">
+        <v>32</v>
+      </c>
+      <c r="W745" t="n">
+        <v>39047.1</v>
+      </c>
+      <c r="X745" t="n">
+        <v>2546</v>
+      </c>
+      <c r="Y745" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z745" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA745" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB745" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC745" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD745" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE745" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF745" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG745" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH745" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI745" t="n">
+        <v>54</v>
+      </c>
+      <c r="AJ745" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK745" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL745" t="inlineStr"/>
+      <c r="AM745" t="inlineStr"/>
+    </row>
+    <row r="746">
+      <c r="A746" s="1" t="n">
+        <v>45335.76219907407</v>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C746" t="n">
+        <v>199.2</v>
+      </c>
+      <c r="D746" t="n">
+        <v>486.1</v>
+      </c>
+      <c r="E746" t="n">
+        <v>200.4</v>
+      </c>
+      <c r="F746" t="n">
+        <v>184.2</v>
+      </c>
+      <c r="G746" t="n">
+        <v>0</v>
+      </c>
+      <c r="H746" t="n">
+        <v>0</v>
+      </c>
+      <c r="I746" t="n">
+        <v>0</v>
+      </c>
+      <c r="J746" t="n">
+        <v>0</v>
+      </c>
+      <c r="K746" t="n">
+        <v>222</v>
+      </c>
+      <c r="L746" t="n">
+        <v>221.4</v>
+      </c>
+      <c r="M746" t="n">
+        <v>223</v>
+      </c>
+      <c r="N746" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="O746" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="P746" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="Q746" t="n">
+        <v>59.89</v>
+      </c>
+      <c r="R746" t="n">
+        <v>59.88</v>
+      </c>
+      <c r="S746" t="n">
+        <v>59.89</v>
+      </c>
+      <c r="T746" t="n">
+        <v>31</v>
+      </c>
+      <c r="U746" t="n">
+        <v>1</v>
+      </c>
+      <c r="V746" t="n">
+        <v>31.8</v>
+      </c>
+      <c r="W746" t="n">
+        <v>39047.1</v>
+      </c>
+      <c r="X746" t="n">
+        <v>2546</v>
+      </c>
+      <c r="Y746" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z746" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA746" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB746" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC746" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD746" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE746" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF746" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG746" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH746" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI746" t="n">
+        <v>54</v>
+      </c>
+      <c r="AJ746" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK746" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL746" t="inlineStr"/>
+      <c r="AM746" t="inlineStr"/>
+    </row>
+    <row r="747">
+      <c r="A747" s="1" t="n">
+        <v>45335.7656712963</v>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C747" t="n">
+        <v>195.7</v>
+      </c>
+      <c r="D747" t="n">
+        <v>438.5</v>
+      </c>
+      <c r="E747" t="n">
+        <v>199.4</v>
+      </c>
+      <c r="F747" t="n">
+        <v>207.6</v>
+      </c>
+      <c r="G747" t="n">
+        <v>0</v>
+      </c>
+      <c r="H747" t="n">
+        <v>0</v>
+      </c>
+      <c r="I747" t="n">
+        <v>0</v>
+      </c>
+      <c r="J747" t="n">
+        <v>0</v>
+      </c>
+      <c r="K747" t="n">
+        <v>221.6</v>
+      </c>
+      <c r="L747" t="n">
+        <v>221</v>
+      </c>
+      <c r="M747" t="n">
+        <v>223.4</v>
+      </c>
+      <c r="N747" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="O747" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="P747" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="Q747" t="n">
+        <v>59.89</v>
+      </c>
+      <c r="R747" t="n">
+        <v>59.89</v>
+      </c>
+      <c r="S747" t="n">
+        <v>59.9</v>
+      </c>
+      <c r="T747" t="n">
+        <v>19</v>
+      </c>
+      <c r="U747" t="n">
+        <v>1</v>
+      </c>
+      <c r="V747" t="n">
+        <v>31.7</v>
+      </c>
+      <c r="W747" t="n">
+        <v>39047.1</v>
+      </c>
+      <c r="X747" t="n">
+        <v>2546</v>
+      </c>
+      <c r="Y747" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z747" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA747" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB747" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC747" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD747" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE747" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF747" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG747" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH747" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI747" t="n">
+        <v>54</v>
+      </c>
+      <c r="AJ747" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK747" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL747" t="inlineStr"/>
+      <c r="AM747" t="inlineStr"/>
+    </row>
+    <row r="748">
+      <c r="A748" s="1" t="n">
+        <v>45335.76914351852</v>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C748" t="n">
+        <v>203.5</v>
+      </c>
+      <c r="D748" t="n">
+        <v>274.3</v>
+      </c>
+      <c r="E748" t="n">
+        <v>206.5</v>
+      </c>
+      <c r="F748" t="n">
+        <v>198.7</v>
+      </c>
+      <c r="G748" t="n">
+        <v>0</v>
+      </c>
+      <c r="H748" t="n">
+        <v>0</v>
+      </c>
+      <c r="I748" t="n">
+        <v>0</v>
+      </c>
+      <c r="J748" t="n">
+        <v>0</v>
+      </c>
+      <c r="K748" t="n">
+        <v>221</v>
+      </c>
+      <c r="L748" t="n">
+        <v>221</v>
+      </c>
+      <c r="M748" t="n">
+        <v>222.6</v>
+      </c>
+      <c r="N748" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="O748" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="P748" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="Q748" t="n">
+        <v>60</v>
+      </c>
+      <c r="R748" t="n">
+        <v>60</v>
+      </c>
+      <c r="S748" t="n">
+        <v>60</v>
+      </c>
+      <c r="T748" t="n">
+        <v>8</v>
+      </c>
+      <c r="U748" t="n">
+        <v>1</v>
+      </c>
+      <c r="V748" t="n">
+        <v>31.4</v>
+      </c>
+      <c r="W748" t="n">
+        <v>39047.1</v>
+      </c>
+      <c r="X748" t="n">
+        <v>2546</v>
+      </c>
+      <c r="Y748" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z748" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA748" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB748" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC748" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD748" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE748" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF748" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG748" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH748" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI748" t="n">
+        <v>54</v>
+      </c>
+      <c r="AJ748" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK748" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL748" t="inlineStr"/>
+      <c r="AM748" t="inlineStr"/>
+    </row>
+    <row r="749">
+      <c r="A749" s="1" t="n">
+        <v>45335.77261574074</v>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="C749" t="n">
+        <v>191.3</v>
+      </c>
+      <c r="D749" t="n">
+        <v>169.1</v>
+      </c>
+      <c r="E749" t="n">
+        <v>161.9</v>
+      </c>
+      <c r="F749" t="n">
+        <v>171.3</v>
+      </c>
+      <c r="G749" t="n">
+        <v>0</v>
+      </c>
+      <c r="H749" t="n">
+        <v>0</v>
+      </c>
+      <c r="I749" t="n">
+        <v>0</v>
+      </c>
+      <c r="J749" t="n">
+        <v>0</v>
+      </c>
+      <c r="K749" t="n">
+        <v>221.8</v>
+      </c>
+      <c r="L749" t="n">
+        <v>222</v>
+      </c>
+      <c r="M749" t="n">
+        <v>223.6</v>
+      </c>
+      <c r="N749" t="n">
+        <v>1</v>
+      </c>
+      <c r="O749" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="P749" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="Q749" t="n">
+        <v>59.98</v>
+      </c>
+      <c r="R749" t="n">
+        <v>59.99</v>
+      </c>
+      <c r="S749" t="n">
+        <v>59.98</v>
+      </c>
+      <c r="T749" t="n">
+        <v>11</v>
+      </c>
+      <c r="U749" t="n">
+        <v>1</v>
+      </c>
+      <c r="V749" t="n">
+        <v>31.3</v>
+      </c>
+      <c r="W749" t="n">
+        <v>39047.1</v>
+      </c>
+      <c r="X749" t="n">
+        <v>2546</v>
+      </c>
+      <c r="Y749" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z749" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA749" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB749" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC749" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD749" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE749" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF749" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG749" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH749" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI749" t="n">
+        <v>54</v>
+      </c>
+      <c r="AJ749" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK749" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL749" t="inlineStr"/>
+      <c r="AM749" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>